<commit_message>
updating the recovery DOC calcs
</commit_message>
<xml_diff>
--- a/sample lists/20230920_TEMPEST_IONS_POOLED_SOURCE.xlsx
+++ b/sample lists/20230920_TEMPEST_IONS_POOLED_SOURCE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/GitHub/TEMPEST-1-porewater/sample lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D3DDA2-02CC-BF42-B489-EA3EFFECED58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA8AF87-CAC0-734C-93B1-8E52957FB4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" activeTab="2" xr2:uid="{6383E3D4-1645-094A-A6AF-68AB1B180534}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Pooled" sheetId="2" r:id="rId2"/>
     <sheet name="Run List" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="101">
   <si>
     <t>Sample Name</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Do we have this sample?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vial Name </t>
   </si>
 </sst>
 </file>
@@ -408,13 +411,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -828,6 +830,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1305,289 +1308,302 @@
     <sortCondition ref="A2:A46"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F394D4F6-EDFB-5B4A-830E-27AC418D6C25}">
-  <dimension ref="A1:B49"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="1" max="2" width="37" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4"/>
+      <c r="C36" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4"/>
+      <c r="C37" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+      <c r="A49" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>